<commit_message>
Update tracker data 2025-07-22 16:59:32
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +480,8 @@
           <t>Read</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-07-21</t>
-        </is>
+      <c r="C2" s="2" t="n">
+        <v>45859</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -489,6 +491,30 @@
       </c>
       <c r="F2" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Read</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 16:59:48
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,30 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:00:48
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:10:26
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,30 +541,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Test2</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:10:29
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,30 +517,6 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>G2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Test1</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:10:36
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,30 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:11:20
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:21:36
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -556,10 +556,10 @@
         <v>45860</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:23:00
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -532,10 +532,10 @@
         <v>45860</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:35:23
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,30 +541,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Test2</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="E5" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:35:28
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,30 +517,6 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>G2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Test1</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="E4" t="n">
-        <v>100</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:35:34
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,30 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Mask1</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:35:43
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Wekk1</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:41:00
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,30 +541,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Wekk1</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:45:58
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,30 +517,6 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>G2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Mask1</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:46:02
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,54 +465,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>G1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Read</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>45859</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>G1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Read</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.04060401</v>
-      </c>
-      <c r="E3" t="n">
-        <v>100</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:55:56
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +469,54 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Read</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>45859</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Read</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 18:01:55
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,54 +465,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>G1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Read</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>45859</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>G1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Read</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="E3" t="n">
-        <v>100</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-20 05:28:46
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +469,30 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>45889</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-20 05:29:28
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,6 +493,30 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45889</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-20 05:47:49
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,1350 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45861</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45862</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9900990099009901</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.9802960494069208</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45864</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.9705901479276444</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45865</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9609803444828162</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45866</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.9514656876067488</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45867</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9420452352542067</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45868</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.9327180547071353</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45869</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.9234832224823122</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45870</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.914339824239913</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45871</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9052869546929831</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45872</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.896323717517805</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45873</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.8874492252651535</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>45874</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.8786625992724292</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45875</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.8699629695766625</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45876</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.8613494748283788</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45877</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.8528212622063156</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>45878</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.8443774873329858</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>45879</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.8360173141910751</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>45880</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.8277399150406684</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.8195444703372954</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>45882</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.8114301686507875</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>45883</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.8033962065849382</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>45884</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.7954417886979586</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>45885</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.7875661274237213</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>45886</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.7797684429937835</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>45887</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.7720479633601817</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>45888</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.7644039241189917</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>45861</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>45862</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.9900990099009901</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>45863</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.9802960494069208</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>45864</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.9705901479276444</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>45865</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.9609803444828162</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>45866</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.9514656876067488</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>45867</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.9420452352542067</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>45868</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.9327180547071353</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>45869</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.9234832224823122</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>45870</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.914339824239913</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>45871</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.9052869546929831</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>45872</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.896323717517805</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>45873</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.8874492252651535</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>45874</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.8786625992724292</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>45875</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.8699629695766625</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>45876</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.8613494748283788</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>45877</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.8528212622063156</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>45878</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.8443774873329858</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>45879</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.8360173141910751</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>45880</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.8277399150406684</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.8195444703372954</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>45882</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.8114301686507875</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>45883</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.8033962065849382</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>45884</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.7954417886979586</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>45885</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.7875661274237213</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>45886</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.7797684429937835</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>45887</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.7720479633601817</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>45888</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.7644039241189917</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-21 00:02:49
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1861,6 +1861,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>45890</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.7568355684346453</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="n">
+        <v>45890</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.7568355684346453</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-22 00:02:49
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1909,6 +1909,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="n">
+        <v>45891</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.7493421469649953</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="n">
+        <v>45891</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.7493421469649953</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-23 00:02:49
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1957,6 +1957,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>45892</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.741922917787124</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="n">
+        <v>45892</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.741922917787124</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-24 00:02:49
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2005,6 +2005,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>45893</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.7345771463238852</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>45893</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.7345771463238852</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-25 00:02:49
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2053,6 +2053,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="n">
+        <v>45894</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.7273041052711734</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>45894</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.7273041052711734</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-08-26 00:02:49
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2101,6 +2101,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>45895</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.7201030745259143</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>45895</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.7201030745259143</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-01 18:04:07
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2149,6 +2149,294 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="n">
+        <v>45896</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.7129733411147666</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="n">
+        <v>45897</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.7059141991235313</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="n">
+        <v>45898</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.6989249496272587</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.6920049006210482</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>45900</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.6851533669515329</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C77" s="2" t="n">
+        <v>45901</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.6783696702490425</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>45896</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.7129733411147666</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="n">
+        <v>45897</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.7059141991235313</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>45898</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.6989249496272587</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.6920049006210482</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>45900</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.6851533669515329</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C83" s="2" t="n">
+        <v>45901</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.6783696702490425</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-02 00:04:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2437,6 +2437,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.6716531388604381</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C85" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.6716531388604381</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-03 00:04:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2485,6 +2485,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.665003107782612</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.665003107782612</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-04 00:04:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2533,6 +2533,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.6584189185966455</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.6584189185966455</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-05 00:04:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2581,6 +2581,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>45905</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.6518999194026193</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="n">
+        <v>45905</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.6518999194026193</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-06 00:04:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2629,6 +2629,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>45906</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.6454454647550686</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C93" s="2" t="n">
+        <v>45906</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.6454454647550686</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-07 00:03:47
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2677,6 +2677,54 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.6390549155990778</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>sedrftgyhuioygtfrd</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.6390549155990778</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-07 16:21:30
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1597,6 +1597,30 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-07 16:21:42
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1621,6 +1621,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-07 16:22:03
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1645,6 +1645,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-07 16:22:24
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1669,6 +1669,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-07 16:22:57
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1693,6 +1693,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>45907</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-08 00:03:47
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,6 +589,126 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45908</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.9900990099009901</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45908</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9900990099009901</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45908</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.9900990099009901</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45908</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9900990099009901</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45908</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.9900990099009901</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-09 00:03:47
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -709,6 +709,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.9802960494069208</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.9802960494069208</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9802960494069208</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9802960494069208</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.9802960494069208</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-10 00:03:47
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -829,6 +829,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.9705901479276444</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.9705901479276444</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.9705901479276444</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.9705901479276444</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.9705901479276444</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-11 00:03:47
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -949,6 +949,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.9609803444828162</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.9609803444828162</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.9609803444828162</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.9609803444828162</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.9609803444828162</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-12 00:03:47
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1069,6 +1069,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.9514656876067488</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.9514656876067488</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.9514656876067488</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.9514656876067488</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.9514656876067488</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-13 00:03:47
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1189,6 +1189,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.9420452352542067</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.9420452352542067</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.9420452352542067</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.9420452352542067</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.9420452352542067</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-14 00:02:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1309,6 +1309,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.9327180547071353</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.9327180547071353</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.9327180547071353</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.9327180547071353</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.9327180547071353</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-15 00:02:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1429,6 +1429,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.9234832224823122</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.9234832224823122</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.9234832224823122</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.9234832224823122</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.9234832224823122</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-16 00:02:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1549,6 +1549,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>45916</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.914339824239913</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>45916</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.914339824239913</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>45916</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.914339824239913</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>45916</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.914339824239913</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>45916</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.914339824239913</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-17 00:02:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1669,6 +1669,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.9052869546929831</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.9052869546929831</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.9052869546929831</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.9052869546929831</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.9052869546929831</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-18 00:02:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1789,6 +1789,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.896323717517805</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.896323717517805</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.896323717517805</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.896323717517805</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.896323717517805</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-19 00:02:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1909,6 +1909,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.8874492252651535</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.8874492252651535</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.8874492252651535</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.8874492252651535</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.8874492252651535</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-20 00:02:05
</commit_message>
<xml_diff>
--- a/progress_history.xlsx
+++ b/progress_history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2029,6 +2029,126 @@
         <v>-0.01</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Workout</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>45920</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.8786625992724292</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Eat Healthy</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="n">
+        <v>45920</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.8786625992724292</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Read Book</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>45920</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.8786625992724292</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Investment Plan</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>45920</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.8786625992724292</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>G6</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Spend 10 Hours without phone</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>45920</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.8786625992724292</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>